<commit_message>
operator page remaining only
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Engineering\Manish\manish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967D4735-7E59-41A8-8D7C-46894D130D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E61819F-C4A0-43D9-86ED-0B6D022473B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>orders</t>
   </si>
   <si>
-    <t>orderdetails</t>
-  </si>
-  <si>
     <t>quantity</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>current</t>
+  </si>
+  <si>
+    <t>measuredValues</t>
   </si>
 </sst>
 </file>
@@ -424,35 +424,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4:U4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -472,49 +478,10 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" t="s">
-        <v>8</v>
-      </c>
-      <c r="P2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S2" t="s">
-        <v>16</v>
-      </c>
-      <c r="T2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U2" t="s">
-        <v>18</v>
-      </c>
-      <c r="V2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -536,64 +503,122 @@
       <c r="G3">
         <v>100</v>
       </c>
-      <c r="I3">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>8.9</v>
+      </c>
+      <c r="D9">
+        <v>9.1</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="K3">
-        <v>8.9</v>
-      </c>
-      <c r="L3">
-        <v>9.1</v>
-      </c>
-      <c r="M3">
+      <c r="C10">
+        <v>2.9</v>
+      </c>
+      <c r="D10">
+        <v>3.1</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1">
+        <v>45749</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17">
         <v>9</v>
       </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R3" s="1">
-        <v>45749</v>
-      </c>
-      <c r="S3" t="s">
-        <v>17</v>
-      </c>
-      <c r="T3">
+      <c r="G17">
         <v>9</v>
       </c>
-      <c r="U3">
-        <v>9</v>
-      </c>
-      <c r="V3" t="b">
+      <c r="H17" t="b">
         <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4">
-        <v>2.9</v>
-      </c>
-      <c r="L4">
-        <v>3.1</v>
-      </c>
-      <c r="M4">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>